<commit_message>
optimize the associate program
</commit_message>
<xml_diff>
--- a/associate/regularNum.xlsx
+++ b/associate/regularNum.xlsx
@@ -403,63 +403,63 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>615</v>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>426</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>286</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>194</v>
       </c>
       <c r="F2">
+        <v>124</v>
+      </c>
+      <c r="G2">
+        <v>61</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>3</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>327</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -467,28 +467,28 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -499,25 +499,25 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -531,25 +531,25 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -563,25 +563,25 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
-        <v>0.6000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -595,25 +595,25 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
-        <v>0.7000000000000001</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -627,25 +627,25 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -659,25 +659,25 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <v>0</v>

</xml_diff>